<commit_message>
Figure 2, version 3
</commit_message>
<xml_diff>
--- a/belize_data/dataset/belize_df.xlsx
+++ b/belize_data/dataset/belize_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\newgdrive\My Drive\Econ PhD\Work 2023\Quota baskets\belize_basket\belize_data\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D91EF3-7EBB-4F2F-9776-45535BDE51D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C761244C-F8C4-4DBE-8C7B-7763DA0078C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{08DB3185-034C-4C09-8288-62234A8608F2}"/>
   </bookViews>
@@ -934,9 +934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A79944D-A632-457E-8222-CE9CE185B041}">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,20 +944,19 @@
     <col min="1" max="1" width="8.88671875" style="4"/>
     <col min="2" max="2" width="20.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" style="4" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="4" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="4" customWidth="1"/>
     <col min="12" max="13" width="8.88671875" style="4"/>
-    <col min="14" max="16" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="8.88671875" style="4" customWidth="1"/>
     <col min="17" max="17" width="8.88671875" style="4"/>
-    <col min="18" max="18" width="12" style="4" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="4" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="4" customWidth="1"/>
     <col min="20" max="22" width="8.88671875" style="4"/>
-    <col min="23" max="24" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="8.88671875" style="4" customWidth="1"/>
     <col min="25" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>

</xml_diff>